<commit_message>
made way too much changes for my own good...
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB28B5CE-EAA1-4649-B6B5-1211C6E5A44E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049911E8-ECC8-46B1-82A3-85A69A498DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="1" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -283,6 +283,66 @@
   </si>
   <si>
     <t>style</t>
+  </si>
+  <si>
+    <t>ingredients</t>
+  </si>
+  <si>
+    <t>allergenes</t>
+  </si>
+  <si>
+    <t>vege ok</t>
+  </si>
+  <si>
+    <t>vegan ok</t>
+  </si>
+  <si>
+    <t>liste des produits</t>
+  </si>
+  <si>
+    <t>liste des ingrédients</t>
+  </si>
+  <si>
+    <t>ajouter ingrédient</t>
+  </si>
+  <si>
+    <t>modifier ingrédient</t>
+  </si>
+  <si>
+    <t>masquer ingrédient</t>
+  </si>
+  <si>
+    <t>supprimer ingrédient</t>
+  </si>
+  <si>
+    <t>liste des catégories</t>
+  </si>
+  <si>
+    <t>ajouter catégorie</t>
+  </si>
+  <si>
+    <t>modifier catégorie</t>
+  </si>
+  <si>
+    <t>masquer catégorie</t>
+  </si>
+  <si>
+    <t>supprimer catégorie</t>
+  </si>
+  <si>
+    <t>admin blog</t>
+  </si>
+  <si>
+    <t>créer un article</t>
+  </si>
+  <si>
+    <t>modifier un article</t>
+  </si>
+  <si>
+    <t>supprimer un article</t>
+  </si>
+  <si>
+    <t>newsletter</t>
   </si>
 </sst>
 </file>
@@ -479,10 +539,6 @@
     </a>
   </bag>
 </FeaturePropertyBags>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -802,10 +858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,16 +1025,16 @@
     <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C9" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="7" t="b">
         <v>0</v>
@@ -990,12 +1046,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="C11" s="7" t="b">
         <v>0</v>
@@ -1019,128 +1097,107 @@
     <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="C16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="C14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="C16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="C18" s="7" t="b">
         <v>0</v>
@@ -1164,131 +1221,152 @@
     <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="C20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="C23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B25" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="C21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G24" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="C26" s="10" t="b">
         <v>0</v>
@@ -1312,7 +1390,7 @@
     <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C27" s="10" t="b">
         <v>0</v>
@@ -1333,12 +1411,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H28" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C29" s="10" t="b">
         <v>0</v>
@@ -1361,98 +1461,522 @@
     </row>
     <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="B30" s="9" t="s">
+    </row>
+    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H33" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="B34" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H34" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H37" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8"/>
+      <c r="B38" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H38" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H39" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C41" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H43" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="B44" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="17"/>
+    </row>
+    <row r="46" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E46" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H46" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
+      <c r="B48" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C48" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8"/>
+      <c r="B51" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="E30" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="F30" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="G30" s="10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H30" s="10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="C51" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+      <c r="B52" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C52" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E52" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="H52" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B54" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="15" t="s">
+      <c r="C54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="14"/>
+      <c r="B55" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="E33" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="H33" s="16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="C55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C35" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G35" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="13" t="b">
+      <c r="C57" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1466,7 +1990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9F86D8-E81A-4260-920D-5D56315E9A1B}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
integrated material theming + sidenav + routing
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049911E8-ECC8-46B1-82A3-85A69A498DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5D64B4-7133-4304-94B4-DA389A1CB41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView minimized="1" xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="11295" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="103">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>newsletter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">temps </t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -505,6 +508,27 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutre" xfId="2" builtinId="28"/>
@@ -858,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:H57"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,9 +894,10 @@
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>74</v>
       </c>
@@ -897,8 +922,11 @@
       <c r="H1" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -923,8 +951,9 @@
       <c r="H3" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6" t="s">
         <v>67</v>
@@ -947,8 +976,9 @@
       <c r="H4" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
         <v>68</v>
@@ -971,8 +1001,9 @@
       <c r="H5" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="24"/>
+    </row>
+    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
@@ -997,8 +1028,9 @@
       <c r="H7" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
         <v>64</v>
@@ -1021,8 +1053,9 @@
       <c r="H8" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>82</v>
@@ -1045,8 +1078,9 @@
       <c r="H9" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
         <v>83</v>
@@ -1069,8 +1103,9 @@
       <c r="H10" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="6" t="s">
         <v>84</v>
@@ -1093,8 +1128,9 @@
       <c r="H11" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>85</v>
@@ -1117,8 +1153,9 @@
       <c r="H12" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>80</v>
@@ -1141,8 +1178,9 @@
       <c r="H13" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="24"/>
+    </row>
+    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>75</v>
       </c>
@@ -1167,8 +1205,9 @@
       <c r="H15" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6" t="s">
         <v>76</v>
@@ -1191,8 +1230,9 @@
       <c r="H16" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="24"/>
+    </row>
+    <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1217,8 +1257,9 @@
       <c r="H18" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
         <v>69</v>
@@ -1241,8 +1282,9 @@
       <c r="H19" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
       <c r="C20" s="19" t="b">
         <v>0</v>
@@ -1262,8 +1304,9 @@
       <c r="H20" s="19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="25"/>
+    </row>
+    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>0</v>
       </c>
@@ -1288,8 +1331,9 @@
       <c r="H21" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6" t="s">
         <v>61</v>
@@ -1312,8 +1356,9 @@
       <c r="H22" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6" t="s">
         <v>62</v>
@@ -1336,8 +1381,9 @@
       <c r="H23" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="24"/>
+    </row>
+    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>3</v>
       </c>
@@ -1362,8 +1408,9 @@
       <c r="H25" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="26"/>
+    </row>
+    <row r="26" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="9" t="s">
         <v>70</v>
@@ -1386,8 +1433,9 @@
       <c r="H26" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="9" t="s">
         <v>71</v>
@@ -1410,8 +1458,9 @@
       <c r="H27" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
         <v>72</v>
@@ -1434,8 +1483,9 @@
       <c r="H28" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="26"/>
+    </row>
+    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8"/>
       <c r="B29" s="9" t="s">
         <v>73</v>
@@ -1458,11 +1508,13 @@
       <c r="H29" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-    </row>
-    <row r="31" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="26"/>
+    </row>
+    <row r="31" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="9" t="s">
         <v>87</v>
@@ -1485,8 +1537,9 @@
       <c r="H31" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="26"/>
+    </row>
+    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="9" t="s">
         <v>88</v>
@@ -1509,8 +1562,9 @@
       <c r="H32" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="9" t="s">
         <v>89</v>
@@ -1533,8 +1587,9 @@
       <c r="H33" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="26"/>
+    </row>
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="9" t="s">
         <v>90</v>
@@ -1557,8 +1612,9 @@
       <c r="H34" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="26"/>
+    </row>
+    <row r="35" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
         <v>91</v>
@@ -1581,11 +1637,13 @@
       <c r="H35" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="26"/>
+    </row>
+    <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
-    </row>
-    <row r="37" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="26"/>
+    </row>
+    <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="9" t="s">
         <v>92</v>
@@ -1608,8 +1666,9 @@
       <c r="H37" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="26"/>
+    </row>
+    <row r="38" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="9" t="s">
         <v>93</v>
@@ -1632,8 +1691,9 @@
       <c r="H38" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="26"/>
+    </row>
+    <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="9" t="s">
         <v>94</v>
@@ -1656,8 +1716,9 @@
       <c r="H39" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="26"/>
+    </row>
+    <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="9" t="s">
         <v>95</v>
@@ -1680,8 +1741,9 @@
       <c r="H40" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="26"/>
+    </row>
+    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="9" t="s">
         <v>96</v>
@@ -1704,8 +1766,9 @@
       <c r="H41" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="26"/>
+    </row>
+    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>4</v>
       </c>
@@ -1730,8 +1793,9 @@
       <c r="H43" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="26"/>
+    </row>
+    <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="9" t="s">
         <v>79</v>
@@ -1754,11 +1818,13 @@
       <c r="H44" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="26"/>
+    </row>
+    <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
-    </row>
-    <row r="46" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="25"/>
+    </row>
+    <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>97</v>
       </c>
@@ -1783,8 +1849,9 @@
       <c r="H46" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="26"/>
+    </row>
+    <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="9" t="s">
         <v>99</v>
@@ -1807,8 +1874,9 @@
       <c r="H47" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="26"/>
+    </row>
+    <row r="48" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="9" t="s">
         <v>100</v>
@@ -1831,9 +1899,10 @@
       <c r="H48" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="26"/>
+    </row>
+    <row r="49" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>5</v>
       </c>
@@ -1858,8 +1927,9 @@
       <c r="H50" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="26"/>
+    </row>
+    <row r="51" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="9" t="s">
         <v>13</v>
@@ -1882,8 +1952,9 @@
       <c r="H51" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="26"/>
+    </row>
+    <row r="52" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="9" t="s">
         <v>101</v>
@@ -1906,8 +1977,9 @@
       <c r="H52" s="10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I52" s="26"/>
+    </row>
+    <row r="54" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>15</v>
       </c>
@@ -1932,8 +2004,9 @@
       <c r="H54" s="16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="28"/>
+    </row>
+    <row r="55" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14"/>
       <c r="B55" s="15" t="s">
         <v>59</v>
@@ -1956,8 +2029,9 @@
       <c r="H55" s="16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="28"/>
+    </row>
+    <row r="57" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>14</v>
       </c>
@@ -1979,6 +2053,7 @@
       <c r="H57" s="13" t="b">
         <v>0</v>
       </c>
+      <c r="I57" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ingredient form works smooth
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3E62EA-ABE6-43DB-BCBE-1D916B822A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AF3B0D-AE16-41D2-9A37-0D4A39AD0368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
@@ -1004,7 +1004,8 @@
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,13 +1220,13 @@
         <v>83</v>
       </c>
       <c r="C10" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="6" t="b">
         <v>0</v>
@@ -1245,13 +1246,13 @@
         <v>84</v>
       </c>
       <c r="C11" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="6" t="b">
         <v>0</v>
@@ -1271,13 +1272,13 @@
         <v>85</v>
       </c>
       <c r="C12" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="6" t="b">
         <v>0</v>
@@ -1671,13 +1672,13 @@
         <v>87</v>
       </c>
       <c r="C31" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="8" t="b">
         <v>0</v>
@@ -1697,13 +1698,13 @@
         <v>88</v>
       </c>
       <c r="C32" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="8" t="b">
         <v>0</v>
@@ -1723,13 +1724,13 @@
         <v>89</v>
       </c>
       <c r="C33" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F33" s="8" t="b">
         <v>0</v>
@@ -1749,13 +1750,13 @@
         <v>90</v>
       </c>
       <c r="C34" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="8" t="b">
         <v>0</v>
@@ -1775,13 +1776,13 @@
         <v>91</v>
       </c>
       <c r="C35" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35" s="8" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
made animated buton for crud ingredient methods
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AF3B0D-AE16-41D2-9A37-0D4A39AD0368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36307C3C-1C2A-41E2-BD68-36B571FA8581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
@@ -1005,7 +1005,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="8" t="b">
         <v>0</v>
@@ -1707,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="8" t="b">
         <v>0</v>
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="8" t="b">
         <v>0</v>
@@ -1750,13 +1750,13 @@
         <v>90</v>
       </c>
       <c r="C34" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="8" t="b">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="8" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
image succesfully deleted when delete its parent object
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36307C3C-1C2A-41E2-BD68-36B571FA8581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E6AD22-87EF-4651-9FDA-EF83616DBB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -309,9 +309,6 @@
     <t>modifier ingrédient</t>
   </si>
   <si>
-    <t>masquer ingrédient</t>
-  </si>
-  <si>
     <t>supprimer ingrédient</t>
   </si>
   <si>
@@ -352,6 +349,18 @@
   </si>
   <si>
     <t>1er clic n'ouvre pas correctement la vue détaillée</t>
+  </si>
+  <si>
+    <t>galerie d'images</t>
+  </si>
+  <si>
+    <t>ajouter une image</t>
+  </si>
+  <si>
+    <t>modifier une image</t>
+  </si>
+  <si>
+    <t>supprimer une image</t>
   </si>
 </sst>
 </file>
@@ -1001,17 +1010,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F35" sqref="F35"/>
+      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="11.42578125" style="11"/>
     <col min="8" max="8" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
@@ -1046,10 +1055,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>102</v>
-      </c>
-      <c r="J1" s="17" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1159,7 +1168,7 @@
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -1558,7 +1567,9 @@
       <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25"/>
+      <c r="A26" s="25">
+        <v>3</v>
+      </c>
       <c r="B26" s="9" t="s">
         <v>70</v>
       </c>
@@ -1667,9 +1678,11 @@
       <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
+      <c r="A31" s="25">
+        <v>2</v>
+      </c>
       <c r="B31" s="9" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C31" s="8" t="b">
         <v>1</v>
@@ -1681,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31" s="8" t="b">
         <v>0</v>
@@ -1695,7 +1708,7 @@
     <row r="32" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="9" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C32" s="8" t="b">
         <v>1</v>
@@ -1707,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="8" t="b">
         <v>0</v>
@@ -1721,7 +1734,7 @@
     <row r="33" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="9" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="C33" s="8" t="b">
         <v>1</v>
@@ -1733,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="8" t="b">
         <v>0</v>
@@ -1747,16 +1760,16 @@
     <row r="34" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="9" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C34" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34" s="8" t="b">
         <v>0</v>
@@ -1772,27 +1785,6 @@
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
-      <c r="B35" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C35" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D35" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F35" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="I35" s="26"/>
       <c r="J35" s="27"/>
     </row>
@@ -1802,21 +1794,23 @@
       <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
+      <c r="A37" s="25">
+        <v>1</v>
+      </c>
       <c r="B37" s="9" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C37" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="8" t="b">
         <v>0</v>
@@ -1830,19 +1824,19 @@
     <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="25"/>
       <c r="B38" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C38" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="8" t="b">
         <v>0</v>
@@ -1856,19 +1850,19 @@
     <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
       <c r="B39" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C39" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="8" t="b">
         <v>0</v>
@@ -1882,19 +1876,19 @@
     <row r="40" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="B40" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C40" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="8" t="b">
         <v>0</v>
@@ -1907,36 +1901,41 @@
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
-      <c r="B41" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C41" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F41" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G41" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H41" s="8" t="b">
-        <v>0</v>
-      </c>
       <c r="I41" s="26"/>
       <c r="J41" s="27"/>
     </row>
+    <row r="42" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="25">
+        <v>4</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
+    </row>
     <row r="43" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
-        <v>4</v>
-      </c>
+      <c r="A43" s="25"/>
       <c r="B43" s="9" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="C43" s="8" t="b">
         <v>0</v>
@@ -1962,7 +1961,7 @@
     <row r="44" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
       <c r="B44" s="9" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="C44" s="8" t="b">
         <v>0</v>
@@ -1985,17 +1984,36 @@
       <c r="I44" s="26"/>
       <c r="J44" s="27"/>
     </row>
-    <row r="45" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="24"/>
+    <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25"/>
+      <c r="B45" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
     </row>
     <row r="46" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="25" t="s">
-        <v>97</v>
-      </c>
+      <c r="A46" s="25"/>
       <c r="B46" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C46" s="8" t="b">
         <v>0</v>
@@ -2018,36 +2036,12 @@
       <c r="I46" s="26"/>
       <c r="J46" s="27"/>
     </row>
-    <row r="47" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D47" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E47" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F47" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G47" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H47" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I47" s="26"/>
-      <c r="J47" s="27"/>
-    </row>
     <row r="48" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25"/>
+      <c r="A48" s="25" t="s">
+        <v>4</v>
+      </c>
       <c r="B48" s="9" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="C48" s="8" t="b">
         <v>0</v>
@@ -2070,39 +2064,43 @@
       <c r="I48" s="26"/>
       <c r="J48" s="27"/>
     </row>
-    <row r="49" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="26"/>
-      <c r="J50" s="27"/>
+    <row r="49" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="25"/>
+      <c r="B49" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="22"/>
+      <c r="I50" s="23"/>
+      <c r="J50" s="24"/>
     </row>
     <row r="51" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25"/>
+      <c r="A51" s="25" t="s">
+        <v>96</v>
+      </c>
       <c r="B51" s="9" t="s">
-        <v>13</v>
+        <v>97</v>
       </c>
       <c r="C51" s="8" t="b">
         <v>0</v>
@@ -2128,7 +2126,7 @@
     <row r="52" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="25"/>
       <c r="B52" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C52" s="8" t="b">
         <v>0</v>
@@ -2151,84 +2149,191 @@
       <c r="I52" s="26"/>
       <c r="J52" s="27"/>
     </row>
-    <row r="54" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="31" t="s">
+    <row r="53" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="25"/>
+      <c r="B53" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E53" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H53" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
+    </row>
+    <row r="54" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27"/>
+    </row>
+    <row r="56" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="25"/>
+      <c r="B56" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E56" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H56" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I56" s="26"/>
+      <c r="J56" s="27"/>
+    </row>
+    <row r="57" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="25"/>
+      <c r="B57" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="26"/>
+      <c r="J57" s="27"/>
+    </row>
+    <row r="59" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B54" s="32" t="s">
+      <c r="B59" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="C54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I54" s="33"/>
-      <c r="J54" s="34"/>
-    </row>
-    <row r="55" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="31"/>
-      <c r="B55" s="32" t="s">
+      <c r="C59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="33"/>
+      <c r="J59" s="34"/>
+    </row>
+    <row r="60" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="31"/>
+      <c r="B60" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G55" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="33"/>
-      <c r="J55" s="34"/>
-    </row>
-    <row r="57" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="C60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="33"/>
+      <c r="J60" s="34"/>
+    </row>
+    <row r="62" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C57" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="37"/>
-      <c r="J57" s="38"/>
+      <c r="C62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" s="37"/>
+      <c r="J62" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished category crud and style
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E6AD22-87EF-4651-9FDA-EF83616DBB9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E1C150-56D8-4D73-A585-A602DF8A56DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="116">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -361,6 +361,76 @@
   </si>
   <si>
     <t>supprimer une image</t>
+  </si>
+  <si>
+    <t>fournisseurs</t>
+  </si>
+  <si>
+    <t>lien avec ingredients</t>
+  </si>
+  <si>
+    <t>alerte</t>
+  </si>
+  <si>
+    <t>télécharger photos</t>
+  </si>
+  <si>
+    <t>1 semaine</t>
+  </si>
+  <si>
+    <t>3 j</t>
+  </si>
+  <si>
+    <r>
+      <t>supression d'un</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="9.9978637043366805E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ingredient </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="9.9978637043366805E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-&gt; affecte produits -&gt; nombre de produits affectés -&gt; confirmation supression</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">supression d'un objet avec </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="3" tint="9.9978637043366805E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>photo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="3" tint="9.9978637043366805E-2"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; proposition dl photos -&gt; confirmation supression</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -519,7 +589,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -656,6 +726,26 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1010,17 +1100,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J62"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A40" sqref="A40:XFD40"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="30" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="11.42578125" style="11"/>
     <col min="8" max="8" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
@@ -1033,7 +1123,7 @@
       <c r="A1" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
@@ -1065,7 +1155,7 @@
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C3" s="6" t="b">
@@ -1091,7 +1181,7 @@
     </row>
     <row r="4" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18"/>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="21" t="s">
         <v>67</v>
       </c>
       <c r="C4" s="6" t="b">
@@ -1117,7 +1207,7 @@
     </row>
     <row r="5" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="21" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="6" t="b">
@@ -1145,7 +1235,7 @@
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C7" s="6" t="b">
@@ -1173,7 +1263,7 @@
     </row>
     <row r="8" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="21" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="6" t="b">
@@ -1199,7 +1289,7 @@
     </row>
     <row r="9" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="21" t="s">
         <v>82</v>
       </c>
       <c r="C9" s="6" t="b">
@@ -1225,7 +1315,7 @@
     </row>
     <row r="10" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="21" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="6" t="b">
@@ -1251,7 +1341,7 @@
     </row>
     <row r="11" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="21" t="s">
         <v>84</v>
       </c>
       <c r="C11" s="6" t="b">
@@ -1277,7 +1367,7 @@
     </row>
     <row r="12" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="21" t="s">
         <v>85</v>
       </c>
       <c r="C12" s="6" t="b">
@@ -1303,7 +1393,7 @@
     </row>
     <row r="13" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="21" t="s">
         <v>80</v>
       </c>
       <c r="C13" s="6" t="b">
@@ -1331,7 +1421,7 @@
       <c r="A15" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="21" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="6" t="b">
@@ -1357,7 +1447,7 @@
     </row>
     <row r="16" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="21" t="s">
         <v>76</v>
       </c>
       <c r="C16" s="6" t="b">
@@ -1385,7 +1475,7 @@
       <c r="A18" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="21" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="6" t="b">
@@ -1411,7 +1501,7 @@
     </row>
     <row r="19" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="21" t="s">
         <v>69</v>
       </c>
       <c r="C19" s="6" t="b">
@@ -1437,6 +1527,7 @@
     </row>
     <row r="20" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="7" t="b">
         <v>0</v>
       </c>
@@ -1462,7 +1553,7 @@
       <c r="A21" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="21" t="s">
         <v>60</v>
       </c>
       <c r="C21" s="6" t="b">
@@ -1488,7 +1579,7 @@
     </row>
     <row r="22" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="21" t="s">
         <v>61</v>
       </c>
       <c r="C22" s="6" t="b">
@@ -1514,7 +1605,7 @@
     </row>
     <row r="23" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="21" t="s">
         <v>62</v>
       </c>
       <c r="C23" s="6" t="b">
@@ -1542,7 +1633,7 @@
       <c r="A25" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="27" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="8" t="b">
@@ -1570,7 +1661,7 @@
       <c r="A26" s="25">
         <v>3</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="27" t="s">
         <v>70</v>
       </c>
       <c r="C26" s="8" t="b">
@@ -1596,7 +1687,7 @@
     </row>
     <row r="27" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C27" s="8" t="b">
@@ -1622,7 +1713,7 @@
     </row>
     <row r="28" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="27" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="8" t="b">
@@ -1648,7 +1739,7 @@
     </row>
     <row r="29" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="27" t="s">
         <v>73</v>
       </c>
       <c r="C29" s="8" t="b">
@@ -1674,6 +1765,7 @@
     </row>
     <row r="30" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
+      <c r="B30" s="27"/>
       <c r="I30" s="26"/>
       <c r="J30" s="27"/>
     </row>
@@ -1681,7 +1773,7 @@
       <c r="A31" s="25">
         <v>2</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="27" t="s">
         <v>104</v>
       </c>
       <c r="C31" s="8" t="b">
@@ -1702,12 +1794,14 @@
       <c r="H31" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="26"/>
+      <c r="I31" s="26" t="s">
+        <v>113</v>
+      </c>
       <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="27" t="s">
         <v>105</v>
       </c>
       <c r="C32" s="8" t="b">
@@ -1733,7 +1827,7 @@
     </row>
     <row r="33" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="27" t="s">
         <v>106</v>
       </c>
       <c r="C33" s="8" t="b">
@@ -1759,7 +1853,7 @@
     </row>
     <row r="34" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="27" t="s">
         <v>107</v>
       </c>
       <c r="C34" s="8" t="b">
@@ -1785,46 +1879,48 @@
     </row>
     <row r="35" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
+      <c r="B35" s="27"/>
       <c r="I35" s="26"/>
       <c r="J35" s="27"/>
     </row>
     <row r="36" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
+      <c r="B36" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H36" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="I36" s="26"/>
       <c r="J36" s="27"/>
     </row>
     <row r="37" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25">
-        <v>1</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C37" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F37" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H37" s="8" t="b">
-        <v>0</v>
-      </c>
+      <c r="A37" s="25"/>
+      <c r="B37" s="27"/>
       <c r="I37" s="26"/>
       <c r="J37" s="27"/>
     </row>
     <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25"/>
-      <c r="B38" s="9" t="s">
-        <v>88</v>
+      <c r="A38" s="25">
+        <v>1</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>87</v>
       </c>
       <c r="C38" s="8" t="b">
         <v>1</v>
@@ -1844,13 +1940,15 @@
       <c r="H38" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="26"/>
+      <c r="I38" s="26" t="s">
+        <v>112</v>
+      </c>
       <c r="J38" s="27"/>
     </row>
     <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
-      <c r="B39" s="9" t="s">
-        <v>89</v>
+      <c r="B39" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="C39" s="8" t="b">
         <v>1</v>
@@ -1875,8 +1973,8 @@
     </row>
     <row r="40" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
-      <c r="B40" s="9" t="s">
-        <v>90</v>
+      <c r="B40" s="27" t="s">
+        <v>89</v>
       </c>
       <c r="C40" s="8" t="b">
         <v>1</v>
@@ -1901,41 +1999,42 @@
     </row>
     <row r="41" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
+      <c r="B41" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F41" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H41" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="I41" s="26"/>
       <c r="J41" s="27"/>
     </row>
     <row r="42" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="25">
-        <v>4</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C42" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G42" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="8" t="b">
-        <v>0</v>
-      </c>
+      <c r="A42" s="25"/>
+      <c r="B42" s="27"/>
       <c r="I42" s="26"/>
       <c r="J42" s="27"/>
     </row>
     <row r="43" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25"/>
-      <c r="B43" s="9" t="s">
-        <v>92</v>
+      <c r="A43" s="25">
+        <v>4</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>91</v>
       </c>
       <c r="C43" s="8" t="b">
         <v>0</v>
@@ -1960,8 +2059,8 @@
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
-      <c r="B44" s="9" t="s">
-        <v>93</v>
+      <c r="B44" s="27" t="s">
+        <v>92</v>
       </c>
       <c r="C44" s="8" t="b">
         <v>0</v>
@@ -1986,8 +2085,8 @@
     </row>
     <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
-      <c r="B45" s="9" t="s">
-        <v>94</v>
+      <c r="B45" s="27" t="s">
+        <v>93</v>
       </c>
       <c r="C45" s="8" t="b">
         <v>0</v>
@@ -2012,8 +2111,8 @@
     </row>
     <row r="46" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
-      <c r="B46" s="9" t="s">
-        <v>95</v>
+      <c r="B46" s="27" t="s">
+        <v>94</v>
       </c>
       <c r="C46" s="8" t="b">
         <v>0</v>
@@ -2036,38 +2135,38 @@
       <c r="I46" s="26"/>
       <c r="J46" s="27"/>
     </row>
-    <row r="48" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="25" t="s">
+    <row r="47" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="25"/>
+      <c r="B47" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H47" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I47" s="26"/>
+      <c r="J47" s="27"/>
+    </row>
+    <row r="49" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B49" s="27" t="s">
         <v>78</v>
-      </c>
-      <c r="C48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" s="26"/>
-      <c r="J48" s="27"/>
-    </row>
-    <row r="49" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
-      <c r="B49" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C49" s="8" t="b">
         <v>0</v>
@@ -2090,43 +2189,44 @@
       <c r="I49" s="26"/>
       <c r="J49" s="27"/>
     </row>
-    <row r="50" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="22"/>
-      <c r="I50" s="23"/>
-      <c r="J50" s="24"/>
-    </row>
-    <row r="51" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+    <row r="50" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="25"/>
+      <c r="B50" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H50" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I50" s="26"/>
+      <c r="J50" s="27"/>
+    </row>
+    <row r="51" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="22"/>
+      <c r="B51" s="24"/>
+      <c r="I51" s="23"/>
+      <c r="J51" s="24"/>
+    </row>
+    <row r="52" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B52" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="C51" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F51" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G51" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
-    </row>
-    <row r="52" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="25"/>
-      <c r="B52" s="9" t="s">
-        <v>98</v>
       </c>
       <c r="C52" s="8" t="b">
         <v>0</v>
@@ -2151,8 +2251,8 @@
     </row>
     <row r="53" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="25"/>
-      <c r="B53" s="9" t="s">
-        <v>99</v>
+      <c r="B53" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="C53" s="8" t="b">
         <v>0</v>
@@ -2175,39 +2275,39 @@
       <c r="I53" s="26"/>
       <c r="J53" s="27"/>
     </row>
-    <row r="54" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="25" t="s">
+    <row r="54" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="25"/>
+      <c r="B54" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I54" s="26"/>
+      <c r="J54" s="27"/>
+    </row>
+    <row r="55" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B56" s="27" t="s">
         <v>12</v>
-      </c>
-      <c r="C55" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F55" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G55" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H55" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I55" s="26"/>
-      <c r="J55" s="27"/>
-    </row>
-    <row r="56" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="25"/>
-      <c r="B56" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="C56" s="8" t="b">
         <v>0</v>
@@ -2232,8 +2332,8 @@
     </row>
     <row r="57" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="25"/>
-      <c r="B57" s="9" t="s">
-        <v>100</v>
+      <c r="B57" s="27" t="s">
+        <v>13</v>
       </c>
       <c r="C57" s="8" t="b">
         <v>0</v>
@@ -2256,38 +2356,38 @@
       <c r="I57" s="26"/>
       <c r="J57" s="27"/>
     </row>
-    <row r="59" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="31" t="s">
+    <row r="58" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="25"/>
+      <c r="B58" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H58" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I58" s="26"/>
+      <c r="J58" s="27"/>
+    </row>
+    <row r="60" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="32" t="s">
+      <c r="B60" s="34" t="s">
         <v>58</v>
-      </c>
-      <c r="C59" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F59" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G59" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H59" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I59" s="33"/>
-      <c r="J59" s="34"/>
-    </row>
-    <row r="60" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="31"/>
-      <c r="B60" s="32" t="s">
-        <v>59</v>
       </c>
       <c r="C60" s="12" t="b">
         <v>0</v>
@@ -2310,30 +2410,144 @@
       <c r="I60" s="33"/>
       <c r="J60" s="34"/>
     </row>
-    <row r="62" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+    <row r="61" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="31"/>
+      <c r="B61" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H61" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I61" s="33"/>
+      <c r="J61" s="34"/>
+    </row>
+    <row r="63" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C62" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D62" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G62" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H62" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I62" s="37"/>
-      <c r="J62" s="38"/>
+      <c r="B63" s="38"/>
+      <c r="C63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" s="37"/>
+      <c r="J63" s="38"/>
+    </row>
+    <row r="64" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="40"/>
+      <c r="B64" s="41"/>
+      <c r="I64" s="42"/>
+      <c r="J64" s="41"/>
+    </row>
+    <row r="65" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="40"/>
+      <c r="B65" s="41"/>
+      <c r="I65" s="42"/>
+      <c r="J65" s="41"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C68" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D68" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E68" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" s="39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B69" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" s="39" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed ingredient and category bugs in product form
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E1C150-56D8-4D73-A585-A602DF8A56DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766D817E-2E54-4CCD-979E-F76624BB2FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -373,9 +373,6 @@
   </si>
   <si>
     <t>télécharger photos</t>
-  </si>
-  <si>
-    <t>1 semaine</t>
   </si>
   <si>
     <t>3 j</t>
@@ -431,6 +428,12 @@
       </rPr>
       <t xml:space="preserve"> -&gt; proposition dl photos -&gt; confirmation supression</t>
     </r>
+  </si>
+  <si>
+    <t>2j</t>
+  </si>
+  <si>
+    <t>2 sem</t>
   </si>
 </sst>
 </file>
@@ -589,7 +592,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -727,25 +730,13 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1103,8 +1094,8 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J31" s="27"/>
     </row>
@@ -1941,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="26" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J38" s="27"/>
     </row>
@@ -2037,16 +2028,16 @@
         <v>91</v>
       </c>
       <c r="C43" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="8" t="b">
         <v>0</v>
@@ -2054,7 +2045,9 @@
       <c r="H43" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="26"/>
+      <c r="I43" s="26" t="s">
+        <v>115</v>
+      </c>
       <c r="J43" s="27"/>
     </row>
     <row r="44" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -2063,16 +2056,16 @@
         <v>92</v>
       </c>
       <c r="C44" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F44" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="8" t="b">
         <v>0</v>
@@ -2089,16 +2082,16 @@
         <v>93</v>
       </c>
       <c r="C45" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="8" t="b">
         <v>0</v>
@@ -2141,16 +2134,16 @@
         <v>95</v>
       </c>
       <c r="C47" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="8" t="b">
         <v>0</v>
@@ -2462,19 +2455,7 @@
       <c r="I63" s="37"/>
       <c r="J63" s="38"/>
     </row>
-    <row r="64" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40"/>
-      <c r="B64" s="41"/>
-      <c r="I64" s="42"/>
-      <c r="J64" s="41"/>
-    </row>
-    <row r="65" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="40"/>
-      <c r="B65" s="41"/>
-      <c r="I65" s="42"/>
-      <c r="J65" s="41"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
         <v>108</v>
       </c>
@@ -2500,12 +2481,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>110</v>
       </c>
       <c r="B68" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C68" s="39" t="b">
         <v>0</v>
@@ -2526,9 +2507,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B69" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C69" s="39" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
added image service on product form, need to test it
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766D817E-2E54-4CCD-979E-F76624BB2FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4978ACF7-5D2E-4ED6-9A3C-958452E53A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -434,6 +434,15 @@
   </si>
   <si>
     <t>2 sem</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>admin -&gt; categories -&gt; il est possible d'ouvrire plusieurs fois la création d'une nouvelle cat</t>
+  </si>
+  <si>
+    <t>admin -&gt; product -&gt; ne peut pas ajouter plusieurs images</t>
   </si>
 </sst>
 </file>
@@ -1091,11 +1100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J69"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I39" sqref="I39"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,6 +2537,19 @@
       </c>
       <c r="H69" s="39" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="B71" s="30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B72" s="30" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added preloaded field on ingredient creation from product form, but find a security issu in ingredient form
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2691CC-5A95-4256-8457-EB36F2A3EE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C35E83B-ECE9-4357-9D0A-4033791F7733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="119">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -439,10 +439,7 @@
     <t>bug</t>
   </si>
   <si>
-    <t>admin -&gt; categories -&gt; il est possible d'ouvrire plusieurs fois la création d'une nouvelle cat</t>
-  </si>
-  <si>
-    <t>admin -&gt; product -&gt; ne peut pas ajouter plusieurs images</t>
+    <t>admin -&gt; db -&gt; empecher un debile de mettre des "." ds la db</t>
   </si>
 </sst>
 </file>
@@ -1100,11 +1097,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2539,17 +2536,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
         <v>117</v>
       </c>
       <c r="B71" s="30" t="s">
         <v>118</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B72" s="30" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned code, fixed category display issues in product form
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C35E83B-ECE9-4357-9D0A-4033791F7733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA10795-809B-41CA-96AC-D5D105895A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -440,6 +440,12 @@
   </si>
   <si>
     <t>admin -&gt; db -&gt; empecher un debile de mettre des "." ds la db</t>
+  </si>
+  <si>
+    <t>productform -&gt; impossbile de select 1 cat</t>
+  </si>
+  <si>
+    <t>productform -&gt; ingredient not found si on annule la créa d'un nouvel ingrédient</t>
   </si>
 </sst>
 </file>
@@ -1097,11 +1103,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,6 +2548,16 @@
       </c>
       <c r="B71" s="30" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B73" s="30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B74" s="30" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated services whith BehaviorSubject features for better fetch
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA10795-809B-41CA-96AC-D5D105895A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10193AFE-D7AF-49A5-8907-6AB9902896FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-29990" yWindow="5800" windowWidth="19180" windowHeight="10060" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="123">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>productform -&gt; ingredient not found si on annule la créa d'un nouvel ingrédient</t>
+  </si>
+  <si>
+    <t>productform -&gt; ne met pas à jour la liste ingredient / catégorie avant ouverture du formulaire</t>
+  </si>
+  <si>
+    <t>productform -&gt; ouvre plusieurs fois le formulaire de création d'ingrédient</t>
   </si>
 </sst>
 </file>
@@ -1103,11 +1109,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J74"/>
+  <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B75" sqref="B75"/>
+      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2549,15 +2555,40 @@
       <c r="B71" s="30" t="s">
         <v>118</v>
       </c>
+      <c r="C71" s="39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B72" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="39" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="30" t="s">
         <v>119</v>
       </c>
+      <c r="C73" s="39" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B74" s="30" t="s">
         <v>120</v>
+      </c>
+      <c r="C74" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B75" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C75" s="39" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleting category done : reassigned to default_category
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E67120-E9C4-41F5-A9DA-2A7707458C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DB8DF0-58E1-4281-B3B7-DA780056DE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29990" yWindow="5800" windowWidth="19180" windowHeight="10060" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -452,6 +452,9 @@
   </si>
   <si>
     <t>productform -&gt; ouvre plusieurs fois le formulaire de création d'ingrédient</t>
+  </si>
+  <si>
+    <t>ne renvoie pas l'erreur quand on créer un produit sui existe déjà en db</t>
   </si>
 </sst>
 </file>
@@ -1109,11 +1112,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J75"/>
+  <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2556,7 +2559,7 @@
         <v>118</v>
       </c>
       <c r="C71" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2564,7 +2567,7 @@
         <v>122</v>
       </c>
       <c r="C72" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2588,7 +2591,12 @@
         <v>121</v>
       </c>
       <c r="C75" s="39" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B76" s="30" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixed for category same named issue
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DB8DF0-58E1-4281-B3B7-DA780056DE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA129A3E-B3A7-40C9-9854-F9E7A1D81C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29990" yWindow="5800" windowWidth="19180" windowHeight="10060" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11295" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1115,8 +1115,8 @@
   <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,6 +2597,9 @@
     <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="30" t="s">
         <v>123</v>
+      </c>
+      <c r="C76" s="39" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
charged ingredients and categories into db, fixed research and filter issues
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA129A3E-B3A7-40C9-9854-F9E7A1D81C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876F7232-60E6-4C62-BDB9-443F7296A1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="11295" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -265,9 +265,6 @@
   </si>
   <si>
     <t>page blog</t>
-  </si>
-  <si>
-    <t>visiteur : blog</t>
   </si>
   <si>
     <t>admin : editeur de texte</t>
@@ -455,6 +452,45 @@
   </si>
   <si>
     <t>ne renvoie pas l'erreur quand on créer un produit sui existe déjà en db</t>
+  </si>
+  <si>
+    <t>Modules Angular &amp; outils recommandés</t>
+  </si>
+  <si>
+    <t>MatTable, MatGridList, MatSelect, MatCheckbox, MatPaginator</t>
+  </si>
+  <si>
+    <t>MatCard, MatGridList, MatCarousel</t>
+  </si>
+  <si>
+    <t>ReactiveFormsModule, Validators, Nodemailer (backend)</t>
+  </si>
+  <si>
+    <t>MatTable, MatFormField, PUT API</t>
+  </si>
+  <si>
+    <t>AuthGuard, JWT Interceptor</t>
+  </si>
+  <si>
+    <t>MatGridList, NgxCarousel, MatList</t>
+  </si>
+  <si>
+    <t>MongoDB (suppliers), GET/POST API, ngx-quill (éditeur texte)</t>
+  </si>
+  <si>
+    <t>page recettes</t>
+  </si>
+  <si>
+    <t>Page recettes (table + gestion admin + affichage visiteurs + vidéo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visiteur :  articles + filtrage </t>
+  </si>
+  <si>
+    <t>MongoDB (recipes), GET/POST API, ngx-quill, intégration YouTube</t>
+  </si>
+  <si>
+    <t>œuf non trouvé à o euf</t>
   </si>
 </sst>
 </file>
@@ -499,7 +535,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -543,6 +579,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +655,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -758,6 +800,26 @@
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+      <extLst>
+        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
+          <xfpb:xfComplement i="0"/>
+        </ext>
+      </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1112,11 +1174,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:K79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,10 +1190,11 @@
     <col min="8" max="8" width="11.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="29"/>
     <col min="10" max="10" width="24.42578125" style="30" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="11"/>
+    <col min="11" max="11" width="37.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>74</v>
       </c>
@@ -1148,7 +1211,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>9</v>
@@ -1157,93 +1220,99 @@
         <v>10</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J1" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="21" t="s">
+      <c r="K1" s="17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="21" t="s">
+      <c r="C3" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+    </row>
+    <row r="4" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="35"/>
+      <c r="B4" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-    </row>
-    <row r="5" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="21" t="s">
+      <c r="C4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+    </row>
+    <row r="5" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35"/>
+      <c r="B5" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="7" spans="1:10" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="37"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="7" spans="1:11" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>57</v>
       </c>
@@ -1257,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="b">
         <v>1</v>
@@ -1270,10 +1339,13 @@
       </c>
       <c r="I7" s="20"/>
       <c r="J7" s="21" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="21" t="s">
         <v>64</v>
@@ -1285,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="6" t="b">
         <v>0</v>
@@ -1298,11 +1370,14 @@
       </c>
       <c r="I8" s="20"/>
       <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C9" s="6" t="b">
         <v>1</v>
@@ -1311,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="6" t="b">
         <v>0</v>
@@ -1324,11 +1399,12 @@
       </c>
       <c r="I9" s="20"/>
       <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="21"/>
+    </row>
+    <row r="10" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C10" s="6" t="b">
         <v>1</v>
@@ -1337,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="6" t="b">
         <v>0</v>
@@ -1350,11 +1426,12 @@
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="21"/>
+    </row>
+    <row r="11" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="6" t="b">
         <v>1</v>
@@ -1363,7 +1440,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="6" t="b">
         <v>0</v>
@@ -1376,11 +1453,12 @@
       </c>
       <c r="I11" s="20"/>
       <c r="J11" s="21"/>
-    </row>
-    <row r="12" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="6" t="b">
         <v>1</v>
@@ -1389,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="6" t="b">
         <v>0</v>
@@ -1402,11 +1480,12 @@
       </c>
       <c r="I12" s="20"/>
       <c r="J12" s="21"/>
-    </row>
-    <row r="13" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="21"/>
+    </row>
+    <row r="13" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="6" t="b">
         <v>0</v>
@@ -1427,146 +1506,140 @@
         <v>0</v>
       </c>
       <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
-    </row>
-    <row r="15" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
+    </row>
+    <row r="15" spans="1:11" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
-    </row>
-    <row r="16" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="21" t="s">
+      <c r="B15" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21"/>
-    </row>
-    <row r="18" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="C15" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="43"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="43"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+    </row>
+    <row r="17" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+    </row>
+    <row r="18" spans="1:11" s="44" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="43"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B20" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="21" t="s">
+      <c r="C20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="21" t="s">
         <v>69</v>
-      </c>
-      <c r="C19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-    </row>
-    <row r="21" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>60</v>
       </c>
       <c r="C21" s="6" t="b">
         <v>0</v>
@@ -1588,131 +1661,138 @@
       </c>
       <c r="I21" s="20"/>
       <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="21" t="s">
+      <c r="K21" s="21" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="23"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+    </row>
+    <row r="24" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35"/>
+      <c r="B24" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="21" t="s">
+      <c r="C24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="25" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="C25" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+    </row>
+    <row r="27" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F25" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="26"/>
-      <c r="J25" s="27"/>
-    </row>
-    <row r="26" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25">
-        <v>3</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C26" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E26" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G26" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="26"/>
-      <c r="J26" s="27"/>
-    </row>
-    <row r="27" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
       <c r="B27" s="27" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C27" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="8" t="b">
         <v>0</v>
@@ -1722,23 +1802,26 @@
       </c>
       <c r="I27" s="26"/>
       <c r="J27" s="27"/>
-    </row>
-    <row r="28" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>3</v>
+      </c>
       <c r="B28" s="27" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C28" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="8" t="b">
         <v>0</v>
@@ -1748,23 +1831,24 @@
       </c>
       <c r="I28" s="26"/>
       <c r="J28" s="27"/>
-    </row>
-    <row r="29" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="27"/>
+    </row>
+    <row r="29" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="8" t="b">
         <v>0</v>
@@ -1774,19 +1858,39 @@
       </c>
       <c r="I29" s="26"/>
       <c r="J29" s="27"/>
-    </row>
-    <row r="30" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
-      <c r="B30" s="27"/>
+      <c r="B30" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H30" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="I30" s="26"/>
       <c r="J30" s="27"/>
-    </row>
-    <row r="31" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25">
-        <v>2</v>
-      </c>
+      <c r="K30" s="27"/>
+    </row>
+    <row r="31" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
       <c r="B31" s="27" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C31" s="8" t="b">
         <v>1</v>
@@ -1798,7 +1902,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="8" t="b">
         <v>0</v>
@@ -1806,41 +1910,23 @@
       <c r="H31" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I31" s="26" t="s">
-        <v>112</v>
-      </c>
+      <c r="I31" s="26"/>
       <c r="J31" s="27"/>
-    </row>
-    <row r="32" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="27"/>
+    </row>
+    <row r="32" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
-      <c r="B32" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C32" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D32" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G32" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="8" t="b">
-        <v>0</v>
-      </c>
+      <c r="B32" s="27"/>
       <c r="I32" s="26"/>
       <c r="J32" s="27"/>
-    </row>
-    <row r="33" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="K32" s="27"/>
+    </row>
+    <row r="33" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25">
+        <v>2</v>
+      </c>
       <c r="B33" s="27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C33" s="8" t="b">
         <v>1</v>
@@ -1860,13 +1946,16 @@
       <c r="H33" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I33" s="26"/>
+      <c r="I33" s="26" t="s">
+        <v>111</v>
+      </c>
       <c r="J33" s="27"/>
-    </row>
-    <row r="34" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K33" s="27"/>
+    </row>
+    <row r="34" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
       <c r="B34" s="27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C34" s="8" t="b">
         <v>1</v>
@@ -1888,26 +1977,48 @@
       </c>
       <c r="I34" s="26"/>
       <c r="J34" s="27"/>
-    </row>
-    <row r="35" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="27"/>
+    </row>
+    <row r="35" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
-      <c r="B35" s="27"/>
+      <c r="B35" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="I35" s="26"/>
       <c r="J35" s="27"/>
-    </row>
-    <row r="36" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="27"/>
+    </row>
+    <row r="36" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
       <c r="B36" s="27" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C36" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F36" s="8" t="b">
         <v>0</v>
@@ -1920,31 +2031,31 @@
       </c>
       <c r="I36" s="26"/>
       <c r="J36" s="27"/>
-    </row>
-    <row r="37" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="27"/>
+    </row>
+    <row r="37" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
       <c r="B37" s="27"/>
       <c r="I37" s="26"/>
       <c r="J37" s="27"/>
-    </row>
-    <row r="38" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="25">
-        <v>1</v>
-      </c>
+      <c r="K37" s="27"/>
+    </row>
+    <row r="38" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="25"/>
       <c r="B38" s="27" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
       <c r="C38" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D38" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38" s="8" t="b">
         <v>0</v>
@@ -1952,41 +2063,23 @@
       <c r="H38" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I38" s="26" t="s">
-        <v>116</v>
-      </c>
+      <c r="I38" s="26"/>
       <c r="J38" s="27"/>
-    </row>
-    <row r="39" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="27"/>
+    </row>
+    <row r="39" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
-      <c r="B39" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F39" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H39" s="8" t="b">
-        <v>0</v>
-      </c>
+      <c r="B39" s="27"/>
       <c r="I39" s="26"/>
       <c r="J39" s="27"/>
-    </row>
-    <row r="40" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="25"/>
+      <c r="K39" s="27"/>
+    </row>
+    <row r="40" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="25">
+        <v>1</v>
+      </c>
       <c r="B40" s="27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C40" s="8" t="b">
         <v>1</v>
@@ -2006,13 +2099,16 @@
       <c r="H40" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I40" s="26"/>
+      <c r="I40" s="26" t="s">
+        <v>115</v>
+      </c>
       <c r="J40" s="27"/>
-    </row>
-    <row r="41" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="27"/>
+    </row>
+    <row r="41" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="B41" s="27" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C41" s="8" t="b">
         <v>1</v>
@@ -2034,19 +2130,39 @@
       </c>
       <c r="I41" s="26"/>
       <c r="J41" s="27"/>
-    </row>
-    <row r="42" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="27"/>
+    </row>
+    <row r="42" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="25"/>
-      <c r="B42" s="27"/>
+      <c r="B42" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F42" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="8" t="b">
+        <v>0</v>
+      </c>
       <c r="I42" s="26"/>
       <c r="J42" s="27"/>
-    </row>
-    <row r="43" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25">
-        <v>4</v>
-      </c>
+      <c r="K42" s="27"/>
+    </row>
+    <row r="43" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="25"/>
       <c r="B43" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C43" s="8" t="b">
         <v>1</v>
@@ -2066,41 +2182,23 @@
       <c r="H43" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I43" s="26" t="s">
-        <v>115</v>
-      </c>
+      <c r="I43" s="26"/>
       <c r="J43" s="27"/>
-    </row>
-    <row r="44" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K43" s="27"/>
+    </row>
+    <row r="44" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
-      <c r="B44" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="C44" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F44" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" s="8" t="b">
-        <v>0</v>
-      </c>
+      <c r="B44" s="27"/>
       <c r="I44" s="26"/>
       <c r="J44" s="27"/>
-    </row>
-    <row r="45" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="25"/>
+      <c r="K44" s="27"/>
+    </row>
+    <row r="45" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="25">
+        <v>4</v>
+      </c>
       <c r="B45" s="27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C45" s="8" t="b">
         <v>1</v>
@@ -2120,25 +2218,28 @@
       <c r="H45" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="I45" s="26"/>
+      <c r="I45" s="26" t="s">
+        <v>114</v>
+      </c>
       <c r="J45" s="27"/>
-    </row>
-    <row r="46" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="27"/>
+    </row>
+    <row r="46" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="B46" s="27" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C46" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="8" t="b">
         <v>0</v>
@@ -2148,11 +2249,12 @@
       </c>
       <c r="I46" s="26"/>
       <c r="J46" s="27"/>
-    </row>
-    <row r="47" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="27"/>
+    </row>
+    <row r="47" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="B47" s="27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C47" s="8" t="b">
         <v>1</v>
@@ -2174,25 +2276,51 @@
       </c>
       <c r="I47" s="26"/>
       <c r="J47" s="27"/>
-    </row>
-    <row r="49" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
-        <v>4</v>
-      </c>
+      <c r="K47" s="27"/>
+    </row>
+    <row r="48" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="25"/>
+      <c r="B48" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H48" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="26"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+    </row>
+    <row r="49" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="25"/>
       <c r="B49" s="27" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="C49" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="8" t="b">
         <v>0</v>
@@ -2202,45 +2330,41 @@
       </c>
       <c r="I49" s="26"/>
       <c r="J49" s="27"/>
-    </row>
-    <row r="50" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="25"/>
-      <c r="B50" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H50" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I50" s="26"/>
-      <c r="J50" s="27"/>
-    </row>
-    <row r="51" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="22"/>
-      <c r="B51" s="24"/>
-      <c r="I51" s="23"/>
-      <c r="J51" s="24"/>
-    </row>
-    <row r="52" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="25" t="s">
-        <v>96</v>
-      </c>
+      <c r="K49" s="27"/>
+    </row>
+    <row r="51" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+    </row>
+    <row r="52" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="25"/>
       <c r="B52" s="27" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="C52" s="8" t="b">
         <v>0</v>
@@ -2262,37 +2386,21 @@
       </c>
       <c r="I52" s="26"/>
       <c r="J52" s="27"/>
-    </row>
-    <row r="53" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="25"/>
-      <c r="B53" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E53" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F53" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G53" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H53" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I53" s="26"/>
-      <c r="J53" s="27"/>
-    </row>
-    <row r="54" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="25"/>
+      <c r="K52" s="27"/>
+    </row>
+    <row r="53" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="22"/>
+      <c r="B53" s="24"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
+    </row>
+    <row r="54" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>95</v>
+      </c>
       <c r="B54" s="27" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C54" s="8" t="b">
         <v>0</v>
@@ -2314,14 +2422,39 @@
       </c>
       <c r="I54" s="26"/>
       <c r="J54" s="27"/>
-    </row>
-    <row r="55" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="25" t="s">
-        <v>5</v>
-      </c>
+      <c r="K54" s="27"/>
+    </row>
+    <row r="55" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="25"/>
+      <c r="B55" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+    </row>
+    <row r="56" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="25"/>
       <c r="B56" s="27" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="C56" s="8" t="b">
         <v>0</v>
@@ -2343,37 +2476,15 @@
       </c>
       <c r="I56" s="26"/>
       <c r="J56" s="27"/>
-    </row>
-    <row r="57" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="25"/>
-      <c r="B57" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E57" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="26"/>
-      <c r="J57" s="27"/>
-    </row>
-    <row r="58" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="25"/>
+      <c r="K56" s="27"/>
+    </row>
+    <row r="57" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="25" t="s">
+        <v>5</v>
+      </c>
       <c r="B58" s="27" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="C58" s="8" t="b">
         <v>0</v>
@@ -2395,211 +2506,279 @@
       </c>
       <c r="I58" s="26"/>
       <c r="J58" s="27"/>
-    </row>
-    <row r="60" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="31" t="s">
+      <c r="K58" s="27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="25"/>
+      <c r="B59" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I59" s="26"/>
+      <c r="J59" s="27"/>
+      <c r="K59" s="27"/>
+    </row>
+    <row r="60" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="25"/>
+      <c r="B60" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D60" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E60" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="26"/>
+      <c r="J60" s="27"/>
+      <c r="K60" s="27"/>
+    </row>
+    <row r="62" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="B60" s="34" t="s">
+      <c r="B62" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D60" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E60" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F60" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G60" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H60" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="33"/>
-      <c r="J60" s="34"/>
-    </row>
-    <row r="61" spans="1:10" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="31"/>
-      <c r="B61" s="34" t="s">
+      <c r="C62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H62" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I62" s="33"/>
+      <c r="J62" s="34"/>
+      <c r="K62" s="34"/>
+    </row>
+    <row r="63" spans="1:11" s="32" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="31"/>
+      <c r="B63" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="E61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="F61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="H61" s="12" t="b">
-        <v>0</v>
-      </c>
-      <c r="I61" s="33"/>
-      <c r="J61" s="34"/>
-    </row>
-    <row r="63" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="35" t="s">
+      <c r="C63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="H63" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="I63" s="33"/>
+      <c r="J63" s="34"/>
+      <c r="K63" s="34"/>
+    </row>
+    <row r="65" spans="1:11" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B63" s="38"/>
-      <c r="C63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="D63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="E63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="F63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H63" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I63" s="37"/>
-      <c r="J63" s="38"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="28" t="s">
+      <c r="B65" s="38"/>
+      <c r="C65" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="D65" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E65" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H65" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I65" s="37"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B69" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="C69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C67" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="D67" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H67" s="39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A68" s="28" t="s">
-        <v>110</v>
-      </c>
-      <c r="B68" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C68" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="D68" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E68" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="F68" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="G68" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" s="39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B69" s="30" t="s">
+      <c r="B70" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="C69" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="D69" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="F69" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="G69" s="39" t="b">
-        <v>0</v>
-      </c>
-      <c r="H69" s="39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="28" t="s">
+      <c r="C70" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D70" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B71" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C71" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D71" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G71" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="H71" s="39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="B71" s="30" t="s">
+      <c r="C73" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B74" s="30" t="s">
+        <v>121</v>
+      </c>
+      <c r="C74" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="C71" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B72" s="30" t="s">
+      <c r="C75" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B76" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="C76" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="B77" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C77" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="B78" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B73" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="C73" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B74" s="30" t="s">
-        <v>120</v>
-      </c>
-      <c r="C74" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="B75" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="C75" s="39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B76" s="30" t="s">
-        <v>123</v>
-      </c>
-      <c r="C76" s="39" t="b">
-        <v>0</v>
+      <c r="C78" s="39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="30" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed produc-form, wip on styling
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\Dev\Angular\les_pates_du_chat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laure\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876F7232-60E6-4C62-BDB9-443F7296A1F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638C4E9A-06D4-4CDD-975E-7725156A54E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30110" yWindow="5680" windowWidth="19420" windowHeight="10300" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11295" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -491,6 +491,9 @@
   </si>
   <si>
     <t>œuf non trouvé à o euf</t>
+  </si>
+  <si>
+    <t>champs catégory et composition ne se colore pas en rouge quand erreur</t>
   </si>
 </sst>
 </file>
@@ -1174,11 +1177,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2647,7 +2650,7 @@
       <c r="J65" s="38"/>
       <c r="K65" s="38"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="28" t="s">
         <v>107</v>
       </c>
@@ -2779,6 +2782,11 @@
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B79" s="30" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B81" s="30" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created carousel for admin part
</commit_message>
<xml_diff>
--- a/tracking avancement.xlsx
+++ b/tracking avancement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laure\Documents\Dev\Angular\les_pates_du_chat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638C4E9A-06D4-4CDD-975E-7725156A54E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34BECFFE-A8B8-4356-9743-3720A8181024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="11295" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4C3FDB4E-D56B-4E0F-BA50-967EEA886A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="139">
   <si>
     <t>page d'accueil</t>
   </si>
@@ -494,6 +494,12 @@
   </si>
   <si>
     <t>champs catégory et composition ne se colore pas en rouge quand erreur</t>
+  </si>
+  <si>
+    <t>afficher alerte si le produit existe déjà avant d'envoyer le formulaire pour éviter de tout perdre si formulaire pasok</t>
+  </si>
+  <si>
+    <t>finir dlc autre : pouvoir définir valeur autre : input text</t>
   </si>
 </sst>
 </file>
@@ -1177,11 +1183,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016D17D2-C411-4CE7-9A17-71FCA775D033}">
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2787,6 +2793,16 @@
     <row r="81" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B81" s="30" t="s">
         <v>136</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="B83" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B85" s="30" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>